<commit_message>
finish the code and add a feature to filter the liftside of other language
</commit_message>
<xml_diff>
--- a/xlsx/政策_政策_intext.xlsx
+++ b/xlsx/政策_政策_intext.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>政策</t>
   </si>
@@ -132,144 +132,6 @@
   </si>
   <si>
     <t>智庫</t>
-  </si>
-  <si>
-    <t>https://cy.wikipedia.org/wiki/Polisi</t>
-  </si>
-  <si>
-    <t>Polisi – 威尔士语</t>
-  </si>
-  <si>
-    <t>https://da.wikipedia.org/wiki/Policy</t>
-  </si>
-  <si>
-    <t>Policy – 丹麦语</t>
-  </si>
-  <si>
-    <t>https://de.wikipedia.org/wiki/Policy</t>
-  </si>
-  <si>
-    <t>Policy – 德语</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Policy</t>
-  </si>
-  <si>
-    <t>Policy – 英语</t>
-  </si>
-  <si>
-    <t>https://es.wikipedia.org/wiki/Pol%C3%ADtica_organizacional</t>
-  </si>
-  <si>
-    <t>Política organizacional – 西班牙语</t>
-  </si>
-  <si>
-    <t>https://fa.wikipedia.org/wiki/%D8%AE%D8%B7_%D9%85%D8%B4%DB%8C</t>
-  </si>
-  <si>
-    <t>خط مشی – 波斯语</t>
-  </si>
-  <si>
-    <t>https://hi.wikipedia.org/wiki/%E0%A4%A8%E0%A5%80%E0%A4%A4%E0%A4%BF</t>
-  </si>
-  <si>
-    <t>नीति – 印地语</t>
-  </si>
-  <si>
-    <t>https://id.wikipedia.org/wiki/Kebijakan</t>
-  </si>
-  <si>
-    <t>Kebijakan – 印度尼西亚语</t>
-  </si>
-  <si>
-    <t>https://it.wikipedia.org/wiki/Policy_(politica)</t>
-  </si>
-  <si>
-    <t>Policy (politica) – 意大利语</t>
-  </si>
-  <si>
-    <t>https://ja.wikipedia.org/wiki/%E6%94%BF%E7%AD%96</t>
-  </si>
-  <si>
-    <t>政策 – 日语</t>
-  </si>
-  <si>
-    <t>https://ko.wikipedia.org/wiki/%EC%A0%95%EC%B1%85</t>
-  </si>
-  <si>
-    <t>정책 – 韩语</t>
-  </si>
-  <si>
-    <t>https://new.wikipedia.org/wiki/%E0%A4%A8%E0%A5%80%E0%A4%A4%E0%A4%BF</t>
-  </si>
-  <si>
-    <t>नीति – 尼瓦尔语</t>
-  </si>
-  <si>
-    <t>https://nl.wikipedia.org/wiki/Beleid</t>
-  </si>
-  <si>
-    <t>Beleid – 荷兰语</t>
-  </si>
-  <si>
-    <t>https://no.wikipedia.org/wiki/Policy</t>
-  </si>
-  <si>
-    <t>Policy – 挪威语</t>
-  </si>
-  <si>
-    <t>https://ru.wikipedia.org/wiki/%D0%9F%D0%BE%D0%BB%D0%B8%D1%82%D0%B8%D0%BA%D0%B0_(%D1%83%D0%BF%D1%80%D0%B0%D0%B2%D0%BB%D0%B5%D0%BD%D0%B8%D0%B5)</t>
-  </si>
-  <si>
-    <t>Политика (управление) – 俄语</t>
-  </si>
-  <si>
-    <t>https://sd.wikipedia.org/wiki/%D9%BE%D8%A7%D9%84%D9%8A%D8%B3%D9%8A</t>
-  </si>
-  <si>
-    <t>پاليسي – 信德语</t>
-  </si>
-  <si>
-    <t>https://si.wikipedia.org/wiki/%E0%B6%B4%E0%B7%8A%E2%80%8D%E0%B6%BB%E0%B6%AD%E0%B7%92%E0%B6%B4%E0%B6%AD%E0%B7%8A%E0%B6%AD%E0%B7%92</t>
-  </si>
-  <si>
-    <t>ප්‍රතිපත්ති – 僧伽罗语</t>
-  </si>
-  <si>
-    <t>https://sn.wikipedia.org/wiki/Gwara_(Humaneja)</t>
-  </si>
-  <si>
-    <t>Gwara (Humaneja) – 绍纳语</t>
-  </si>
-  <si>
-    <t>https://sv.wikipedia.org/wiki/Policy</t>
-  </si>
-  <si>
-    <t>Policy – 瑞典语</t>
-  </si>
-  <si>
-    <t>https://ur.wikipedia.org/wiki/%D8%AD%DA%A9%D9%85%D8%AA_%D8%B9%D9%85%D9%84%DB%8C</t>
-  </si>
-  <si>
-    <t>حکمت عملی – 乌尔都语</t>
-  </si>
-  <si>
-    <t>https://vi.wikipedia.org/wiki/Ch%C3%ADnh_s%C3%A1ch</t>
-  </si>
-  <si>
-    <t>Chính sách – 越南语</t>
-  </si>
-  <si>
-    <t>https://yi.wikipedia.org/wiki/%D7%A4%D7%90%D7%9C%D7%99%D7%A1%D7%99</t>
-  </si>
-  <si>
-    <t>פאליסי – 意第绪语</t>
-  </si>
-  <si>
-    <t>https://zh-min-nan.wikipedia.org/wiki/Ch%C3%A8ng-chhek</t>
-  </si>
-  <si>
-    <t>Chèng-chhek – Chinese (Min Nan)</t>
   </si>
 </sst>
 </file>
@@ -618,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1174,673 +1036,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" t="n">
-        <v>19</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="n">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>21</v>
-      </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" t="n">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" t="n">
-        <v>22</v>
-      </c>
-      <c r="E23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" t="n">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" t="n">
-        <v>23</v>
-      </c>
-      <c r="E24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" t="n">
-        <v>24</v>
-      </c>
-      <c r="E25" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" t="n">
-        <v>25</v>
-      </c>
-      <c r="E26" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1</v>
-      </c>
-      <c r="H26" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="n">
-        <v>26</v>
-      </c>
-      <c r="E27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" t="n">
-        <v>27</v>
-      </c>
-      <c r="E28" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" t="s">
-        <v>56</v>
-      </c>
-      <c r="G28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" t="n">
-        <v>28</v>
-      </c>
-      <c r="E29" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" t="s">
-        <v>58</v>
-      </c>
-      <c r="G29" t="n">
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" t="n">
-        <v>29</v>
-      </c>
-      <c r="E30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" t="s">
-        <v>60</v>
-      </c>
-      <c r="G30" t="n">
-        <v>1</v>
-      </c>
-      <c r="H30" t="s">
-        <v>4</v>
-      </c>
-      <c r="I30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" t="n">
-        <v>30</v>
-      </c>
-      <c r="E31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" t="s">
-        <v>62</v>
-      </c>
-      <c r="G31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H31" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" t="n">
-        <v>31</v>
-      </c>
-      <c r="E32" t="s">
-        <v>63</v>
-      </c>
-      <c r="F32" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" t="n">
-        <v>1</v>
-      </c>
-      <c r="H32" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" t="n">
-        <v>32</v>
-      </c>
-      <c r="E33" t="s">
-        <v>65</v>
-      </c>
-      <c r="F33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G33" t="n">
-        <v>1</v>
-      </c>
-      <c r="H33" t="s">
-        <v>4</v>
-      </c>
-      <c r="I33" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" t="n">
-        <v>33</v>
-      </c>
-      <c r="E34" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" t="n">
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
-        <v>4</v>
-      </c>
-      <c r="I34" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" t="n">
-        <v>34</v>
-      </c>
-      <c r="E35" t="s">
-        <v>69</v>
-      </c>
-      <c r="F35" t="s">
-        <v>70</v>
-      </c>
-      <c r="G35" t="n">
-        <v>1</v>
-      </c>
-      <c r="H35" t="s">
-        <v>4</v>
-      </c>
-      <c r="I35" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" t="n">
-        <v>35</v>
-      </c>
-      <c r="E36" t="s">
-        <v>71</v>
-      </c>
-      <c r="F36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G36" t="n">
-        <v>1</v>
-      </c>
-      <c r="H36" t="s">
-        <v>4</v>
-      </c>
-      <c r="I36" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" t="n">
-        <v>36</v>
-      </c>
-      <c r="E37" t="s">
-        <v>73</v>
-      </c>
-      <c r="F37" t="s">
-        <v>74</v>
-      </c>
-      <c r="G37" t="n">
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
-        <v>4</v>
-      </c>
-      <c r="I37" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" t="n">
-        <v>37</v>
-      </c>
-      <c r="E38" t="s">
-        <v>75</v>
-      </c>
-      <c r="F38" t="s">
-        <v>76</v>
-      </c>
-      <c r="G38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" t="s">
-        <v>4</v>
-      </c>
-      <c r="I38" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" t="n">
-        <v>38</v>
-      </c>
-      <c r="E39" t="s">
-        <v>77</v>
-      </c>
-      <c r="F39" t="s">
-        <v>78</v>
-      </c>
-      <c r="G39" t="n">
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
-        <v>4</v>
-      </c>
-      <c r="I39" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" t="n">
-        <v>39</v>
-      </c>
-      <c r="E40" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" t="s">
-        <v>80</v>
-      </c>
-      <c r="G40" t="n">
-        <v>1</v>
-      </c>
-      <c r="H40" t="s">
-        <v>4</v>
-      </c>
-      <c r="I40" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" t="n">
-        <v>40</v>
-      </c>
-      <c r="E41" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" t="s">
-        <v>82</v>
-      </c>
-      <c r="G41" t="n">
-        <v>1</v>
-      </c>
-      <c r="H41" t="s">
-        <v>4</v>
-      </c>
-      <c r="I41" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" t="n">
-        <v>41</v>
-      </c>
-      <c r="E42" t="s">
-        <v>83</v>
-      </c>
-      <c r="F42" t="s">
-        <v>84</v>
-      </c>
-      <c r="G42" t="n">
-        <v>1</v>
-      </c>
-      <c r="H42" t="s">
-        <v>4</v>
-      </c>
-      <c r="I42" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>